<commit_message>
empezado sección 4.3.2.3.1 Reports
Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/PermisosTestDataSportBook.xlsx
+++ b/Data Files/TestData/PermisosTestDataSportBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="93">
   <si>
     <t xml:space="preserve">TestCaseId</t>
   </si>
@@ -287,6 +287,18 @@
   </si>
   <si>
     <t>13:26:16.727</t>
+  </si>
+  <si>
+    <t>15:45:22.137</t>
+  </si>
+  <si>
+    <t>15:45:57.673</t>
+  </si>
+  <si>
+    <t>15:46:53.216</t>
+  </si>
+  <si>
+    <t>15:47:28.370</t>
   </si>
 </sst>
 </file>
@@ -564,13 +576,13 @@
         <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
         <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
         <v>65</v>
@@ -585,10 +597,10 @@
         <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>